<commit_message>
Tried to understand meandiff in tukey results dataframe
I calculated the mean Km for BX across the different vegetation types and subtracted each mean from the other to see how they match up with the meandiff in the results dataframe. Seems like meandiff is calculated by subtracting the mean of group 1 from the mean of group 2
</commit_message>
<xml_diff>
--- a/Statistical analyses/Tukey posthoc/AP/Vmax, timePoint.xlsx
+++ b/Statistical analyses/Tukey posthoc/AP/Vmax, timePoint.xlsx
@@ -16,25 +16,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">group1 group2 meandiff p-adj lower upper reject </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 3 0.5953 0.0667 -0.0285 1.2192 False </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 5 0.0288 0.9 -0.5951 0.6526 False </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 6 -0.254 0.6835 -0.8778 0.3699 False </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 5 -0.5666 0.0879 -1.1904 0.0573 False </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 6 -0.8493 0.0036 -1.4731 -0.2254 True </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 6 -0.2827 0.616 -0.9066 0.3411 False </t>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>meandiff</t>
+  </si>
+  <si>
+    <t>p-adj</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>reject</t>
   </si>
 </sst>
 </file>
@@ -392,45 +392,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0.5953000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.0667</v>
+      </c>
+      <c r="E2">
+        <v>-0.0285</v>
+      </c>
+      <c r="F2">
+        <v>1.2192</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0.0288</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>-0.5951</v>
+      </c>
+      <c r="F3">
+        <v>0.6526</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>-0.254</v>
+      </c>
+      <c r="D4">
+        <v>0.6835</v>
+      </c>
+      <c r="E4">
+        <v>-0.8778</v>
+      </c>
+      <c r="F4">
+        <v>0.3699</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>-0.5666</v>
+      </c>
+      <c r="D5">
+        <v>0.08790000000000001</v>
+      </c>
+      <c r="E5">
+        <v>-1.1904</v>
+      </c>
+      <c r="F5">
+        <v>0.0573</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>-0.8493000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.0036</v>
+      </c>
+      <c r="E6">
+        <v>-1.4731</v>
+      </c>
+      <c r="F6">
+        <v>-0.2254</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>-0.2827</v>
+      </c>
+      <c r="D7">
+        <v>0.616</v>
+      </c>
+      <c r="E7">
+        <v>-0.9066</v>
+      </c>
+      <c r="F7">
+        <v>0.3411</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>